<commit_message>
minor board / part changes
</commit_message>
<xml_diff>
--- a/nixie-tube-clock-hw/fab/nixie-tube-clock digikey.xlsx
+++ b/nixie-tube-clock-hw/fab/nixie-tube-clock digikey.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caden\Documents\GitHub\nixie-tube-clock\nixie-tube-clock-hw\fab\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83559827-235E-4231-B115-CDCA963CFD63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1 - nixie-tube-clock" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet 1 - nixie-tube-clock" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
   <si>
     <t>nixie-tube-clock</t>
   </si>
@@ -191,9 +200,6 @@
   </si>
   <si>
     <t>R5</t>
-  </si>
-  <si>
-    <t>RT0805FRE07180KL</t>
   </si>
   <si>
     <t>R6</t>
@@ -319,10 +325,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2">
     <font>
       <sz val="10"/>
@@ -368,28 +371,28 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -399,23 +402,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffa5a5a5"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFA5A5A5"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Blank">
   <a:themeElements>
     <a:clrScheme name="Blank">
       <a:dk1>
@@ -614,7 +679,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -633,7 +698,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1200" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -663,7 +728,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -689,7 +754,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -715,7 +780,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -741,7 +806,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -767,7 +832,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -793,7 +858,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -819,7 +884,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -845,7 +910,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -871,7 +936,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -884,9 +949,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -903,7 +974,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -922,7 +993,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -948,7 +1019,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -974,7 +1045,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1000,7 +1071,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1026,7 +1097,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1052,7 +1123,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1078,7 +1149,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1104,7 +1175,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1130,7 +1201,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1156,7 +1227,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1169,9 +1240,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1185,7 +1262,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1204,7 +1281,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1234,7 +1311,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1260,7 +1337,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1286,7 +1363,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1312,7 +1389,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1338,7 +1415,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1364,7 +1441,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1390,7 +1467,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1416,7 +1493,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1442,7 +1519,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1455,586 +1532,594 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:C51"/>
+  <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.33333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.28515625" defaultRowHeight="19.899999999999999" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="4.17188" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7891" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.3516" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.35156" style="1" customWidth="1"/>
+    <col min="1" max="1" width="4.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="27.65" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:3" ht="27.6" customHeight="1">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-    </row>
-    <row r="2" ht="20.05" customHeight="1">
-      <c r="A2" t="s" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s" s="3">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+    </row>
+    <row r="2" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s" s="3">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" ht="20.05" customHeight="1">
-      <c r="A3" s="4">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s" s="3">
+    <row r="3" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s" s="3">
+      <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" s="4">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s" s="3">
+    <row r="4" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A4" s="3">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="s" s="3">
+      <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" s="4">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s" s="3">
+    <row r="5" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A5" s="3">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C5" t="s" s="3">
+      <c r="C5" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" s="4">
-        <v>1</v>
-      </c>
-      <c r="B6" t="s" s="3">
+    <row r="6" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A6" s="3">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C6" t="s" s="3">
+      <c r="C6" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" s="4">
+    <row r="7" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A7" s="3">
         <v>4</v>
       </c>
-      <c r="B7" t="s" s="3">
+      <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C7" t="s" s="3">
+      <c r="C7" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" s="4">
-        <v>1</v>
-      </c>
-      <c r="B8" t="s" s="3">
+    <row r="8" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A8" s="3">
+        <v>1</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C8" t="s" s="3">
+      <c r="C8" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="4">
-        <v>1</v>
-      </c>
-      <c r="B9" t="s" s="3">
+    <row r="9" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A9" s="3">
+        <v>1</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C9" t="s" s="3">
+      <c r="C9" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="4">
+    <row r="10" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A10" s="3">
         <v>6</v>
       </c>
-      <c r="B10" t="s" s="3">
+      <c r="B10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C10" t="s" s="3">
+      <c r="C10" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" s="4">
+    <row r="11" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A11" s="3">
         <v>2</v>
       </c>
-      <c r="B11" t="s" s="3">
+      <c r="B11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C11" t="s" s="3">
+      <c r="C11" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" s="4">
+    <row r="12" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A12" s="3">
         <v>8</v>
       </c>
-      <c r="B12" t="s" s="3">
+      <c r="B12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C12" t="s" s="3">
+      <c r="C12" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" ht="20.05" customHeight="1">
-      <c r="A13" s="4">
-        <v>1</v>
-      </c>
-      <c r="B13" t="s" s="3">
+    <row r="13" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A13" s="3">
+        <v>1</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C13" t="s" s="3">
+      <c r="C13" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" ht="20.05" customHeight="1">
-      <c r="A14" s="4">
-        <v>1</v>
-      </c>
-      <c r="B14" t="s" s="3">
+    <row r="14" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A14" s="3">
+        <v>1</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C14" t="s" s="3">
+      <c r="C14" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" s="4">
-        <v>1</v>
-      </c>
-      <c r="B15" t="s" s="3">
+    <row r="15" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A15" s="3">
+        <v>1</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C15" t="s" s="3">
+      <c r="C15" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" ht="20.05" customHeight="1">
-      <c r="A16" s="4">
+    <row r="16" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A16" s="3">
         <v>2</v>
       </c>
-      <c r="B16" t="s" s="3">
+      <c r="B16" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C16" t="s" s="3">
+      <c r="C16" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" s="4">
+    <row r="17" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A17" s="3">
         <v>2</v>
       </c>
-      <c r="B17" t="s" s="3">
+      <c r="B17" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C17" t="s" s="3">
+      <c r="C17" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="18" ht="20.05" customHeight="1">
-      <c r="A18" s="4">
-        <v>1</v>
-      </c>
-      <c r="B18" t="s" s="3">
+    <row r="18" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A18" s="3">
+        <v>1</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C18" t="s" s="3">
+      <c r="C18" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" ht="20.05" customHeight="1">
-      <c r="A19" s="4">
+    <row r="19" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A19" s="3">
         <v>4</v>
       </c>
-      <c r="B19" s="5"/>
-      <c r="C19" t="s" s="3">
+      <c r="B19" s="4"/>
+      <c r="C19" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" s="4">
-        <v>1</v>
-      </c>
-      <c r="B20" t="s" s="3">
+    <row r="20" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A20" s="3">
+        <v>1</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C20" t="s" s="3">
+      <c r="C20" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" s="4">
+    <row r="21" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A21" s="3">
         <v>4</v>
       </c>
-      <c r="B21" t="s" s="3">
+      <c r="B21" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C21" t="s" s="3">
+      <c r="C21" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="22" ht="20.05" customHeight="1">
-      <c r="A22" s="4">
-        <v>1</v>
-      </c>
-      <c r="B22" t="s" s="3">
+    <row r="22" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A22" s="3">
+        <v>1</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C22" t="s" s="3">
+      <c r="C22" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="23" ht="20.05" customHeight="1">
-      <c r="A23" s="4">
-        <v>1</v>
-      </c>
-      <c r="B23" t="s" s="3">
+    <row r="23" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A23" s="3">
+        <v>1</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C23" t="s" s="3">
+      <c r="C23" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="24" ht="20.05" customHeight="1">
-      <c r="A24" s="4">
-        <v>1</v>
-      </c>
-      <c r="B24" t="s" s="3">
+    <row r="24" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A24" s="3">
+        <v>1</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C24" t="s" s="3">
+      <c r="C24" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" ht="20.05" customHeight="1">
-      <c r="A25" s="4">
+    <row r="25" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A25" s="3">
         <v>44</v>
       </c>
-      <c r="B25" t="s" s="3">
+      <c r="B25" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C25" t="s" s="3">
+      <c r="C25" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="26" ht="20.05" customHeight="1">
-      <c r="A26" s="4">
+    <row r="26" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A26" s="3">
         <v>4</v>
       </c>
-      <c r="B26" t="s" s="3">
+      <c r="B26" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C26" t="s" s="3">
+      <c r="C26" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="27" ht="20.05" customHeight="1">
-      <c r="A27" s="4">
-        <v>1</v>
-      </c>
-      <c r="B27" t="s" s="3">
+    <row r="27" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A27" s="3">
+        <v>1</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C27" t="s" s="3">
+      <c r="C27" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="28" ht="20.05" customHeight="1">
-      <c r="A28" s="4">
-        <v>1</v>
-      </c>
-      <c r="B28" t="s" s="3">
+    <row r="28" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A28" s="3">
+        <v>1</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C28" t="s" s="3">
+      <c r="C28" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="29" ht="20.05" customHeight="1">
-      <c r="A29" s="4">
-        <v>1</v>
-      </c>
-      <c r="B29" t="s" s="3">
+    <row r="29" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A29" s="3">
+        <v>1</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C29" t="s" s="3">
+      <c r="C29" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="30" ht="20.05" customHeight="1">
-      <c r="A30" s="4">
-        <v>1</v>
-      </c>
-      <c r="B30" t="s" s="3">
+    <row r="30" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A30" s="3">
+        <v>1</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C30" t="s" s="3">
+      <c r="C30" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="31" ht="20.05" customHeight="1">
-      <c r="A31" s="4">
-        <v>1</v>
-      </c>
-      <c r="B31" t="s" s="3">
+    <row r="31" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A31" s="3">
+        <v>1</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C31" t="s" s="3">
+      <c r="C31" s="2"/>
+    </row>
+    <row r="32" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A32" s="3">
+        <v>1</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="32" ht="20.05" customHeight="1">
-      <c r="A32" s="4">
-        <v>1</v>
-      </c>
-      <c r="B32" t="s" s="3">
+      <c r="C32" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C32" t="s" s="3">
+    </row>
+    <row r="33" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A33" s="3">
+        <v>1</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="33" ht="20.05" customHeight="1">
-      <c r="A33" s="4">
-        <v>1</v>
-      </c>
-      <c r="B33" t="s" s="3">
+      <c r="C33" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C33" t="s" s="3">
+    </row>
+    <row r="34" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A34" s="3">
+        <v>1</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="34" ht="20.05" customHeight="1">
-      <c r="A34" s="4">
-        <v>1</v>
-      </c>
-      <c r="B34" t="s" s="3">
+      <c r="C34" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C34" t="s" s="3">
+    </row>
+    <row r="35" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A35" s="3">
+        <v>3</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="35" ht="20.05" customHeight="1">
-      <c r="A35" s="4">
-        <v>3</v>
-      </c>
-      <c r="B35" t="s" s="3">
+      <c r="C35" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C35" t="s" s="3">
+    </row>
+    <row r="36" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A36" s="3">
+        <v>6</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="36" ht="20.05" customHeight="1">
-      <c r="A36" s="4">
-        <v>6</v>
-      </c>
-      <c r="B36" t="s" s="3">
+      <c r="C36" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C36" t="s" s="3">
+    </row>
+    <row r="37" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A37" s="3">
+        <v>13</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="37" ht="20.05" customHeight="1">
-      <c r="A37" s="4">
-        <v>13</v>
-      </c>
-      <c r="B37" t="s" s="3">
+      <c r="C37" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C37" t="s" s="3">
+    </row>
+    <row r="38" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A38" s="3">
+        <v>2</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="38" ht="20.05" customHeight="1">
-      <c r="A38" s="4">
+      <c r="C38" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A39" s="3">
+        <v>40</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A40" s="3">
+        <v>4</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A41" s="3">
+        <v>4</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A42" s="3">
+        <v>4</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A43" s="3">
+        <v>4</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A44" s="3">
+        <v>4</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A45" s="3">
+        <v>1</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A46" s="3">
+        <v>1</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A47" s="3">
+        <v>1</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A48" s="3">
+        <v>1</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A49" s="3">
+        <v>8</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A50" s="3">
+        <v>1</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A51" s="3">
         <v>2</v>
       </c>
-      <c r="B38" t="s" s="3">
-        <v>73</v>
-      </c>
-      <c r="C38" t="s" s="3">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="39" ht="20.05" customHeight="1">
-      <c r="A39" s="4">
-        <v>40</v>
-      </c>
-      <c r="B39" t="s" s="3">
-        <v>75</v>
-      </c>
-      <c r="C39" t="s" s="3">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="40" ht="20.05" customHeight="1">
-      <c r="A40" s="4">
-        <v>4</v>
-      </c>
-      <c r="B40" t="s" s="3">
-        <v>77</v>
-      </c>
-      <c r="C40" t="s" s="3">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="41" ht="20.05" customHeight="1">
-      <c r="A41" s="4">
-        <v>4</v>
-      </c>
-      <c r="B41" t="s" s="3">
-        <v>79</v>
-      </c>
-      <c r="C41" t="s" s="3">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="42" ht="20.05" customHeight="1">
-      <c r="A42" s="4">
-        <v>4</v>
-      </c>
-      <c r="B42" t="s" s="3">
-        <v>81</v>
-      </c>
-      <c r="C42" t="s" s="3">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="43" ht="20.05" customHeight="1">
-      <c r="A43" s="4">
-        <v>4</v>
-      </c>
-      <c r="B43" t="s" s="3">
-        <v>83</v>
-      </c>
-      <c r="C43" t="s" s="3">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="44" ht="20.05" customHeight="1">
-      <c r="A44" s="4">
-        <v>4</v>
-      </c>
-      <c r="B44" t="s" s="3">
-        <v>85</v>
-      </c>
-      <c r="C44" t="s" s="3">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="45" ht="20.05" customHeight="1">
-      <c r="A45" s="4">
-        <v>1</v>
-      </c>
-      <c r="B45" t="s" s="3">
-        <v>87</v>
-      </c>
-      <c r="C45" t="s" s="3">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="46" ht="20.05" customHeight="1">
-      <c r="A46" s="4">
-        <v>1</v>
-      </c>
-      <c r="B46" t="s" s="3">
-        <v>89</v>
-      </c>
-      <c r="C46" t="s" s="3">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="47" ht="20.05" customHeight="1">
-      <c r="A47" s="4">
-        <v>1</v>
-      </c>
-      <c r="B47" t="s" s="3">
-        <v>91</v>
-      </c>
-      <c r="C47" t="s" s="3">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="48" ht="20.05" customHeight="1">
-      <c r="A48" s="4">
-        <v>1</v>
-      </c>
-      <c r="B48" t="s" s="3">
-        <v>93</v>
-      </c>
-      <c r="C48" t="s" s="3">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="49" ht="20.05" customHeight="1">
-      <c r="A49" s="4">
-        <v>8</v>
-      </c>
-      <c r="B49" t="s" s="3">
-        <v>95</v>
-      </c>
-      <c r="C49" t="s" s="3">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="50" ht="20.05" customHeight="1">
-      <c r="A50" s="4">
-        <v>1</v>
-      </c>
-      <c r="B50" t="s" s="3">
-        <v>97</v>
-      </c>
-      <c r="C50" t="s" s="3">
+      <c r="B51" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="51" ht="20.05" customHeight="1">
-      <c r="A51" s="4">
-        <v>2</v>
-      </c>
-      <c r="B51" t="s" s="3">
+      <c r="C51" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="C51" t="s" s="3">
-        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -2042,7 +2127,7 @@
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>